<commit_message>
Drop tenure_type_label for imports and exports
</commit_message>
<xml_diff>
--- a/cadasta/organization/tests/files/test_conditionals.xlsx
+++ b/cadasta/organization/tests/files/test_conditionals.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>id</t>
   </si>
@@ -105,25 +105,16 @@
     <t>tenure_type</t>
   </si>
   <si>
-    <t>tenure_type_label</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
     <t>CU</t>
   </si>
   <si>
-    <t>Customary Rights</t>
-  </si>
-  <si>
     <t>Some notes</t>
   </si>
   <si>
     <t>WR</t>
-  </si>
-  <si>
-    <t>Water Rights</t>
   </si>
   <si>
     <t>Some more notes</t>
@@ -206,7 +197,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -377,13 +368,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -482,10 +467,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -740,13 +725,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1059,10 +1038,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1602,7 +1581,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1611,9 +1590,8 @@
     <col min="1" max="1" width="27.3516" style="7" customWidth="1"/>
     <col min="2" max="2" width="29.5" style="7" customWidth="1"/>
     <col min="3" max="3" width="19.6719" style="7" customWidth="1"/>
-    <col min="4" max="4" width="19" style="7" customWidth="1"/>
-    <col min="5" max="5" width="8.5" style="7" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="7" customWidth="1"/>
+    <col min="4" max="4" width="8.5" style="7" customWidth="1"/>
+    <col min="5" max="256" width="8.85156" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -1629,9 +1607,6 @@
       <c r="D1" t="s" s="2">
         <v>30</v>
       </c>
-      <c r="E1" t="s" s="2">
-        <v>31</v>
-      </c>
     </row>
     <row r="2" ht="15" customHeight="1">
       <c r="A2" t="s" s="2">
@@ -1641,13 +1616,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s" s="2">
         <v>32</v>
-      </c>
-      <c r="D2" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s" s="2">
-        <v>34</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
@@ -1658,13 +1630,10 @@
         <v>8</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s" s="2">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
@@ -1672,49 +1641,42 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
     </row>
     <row r="5" ht="15" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
     </row>
     <row r="6" ht="15" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
     </row>
     <row r="7" ht="15" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
     </row>
     <row r="8" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
     </row>
     <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
     </row>
     <row r="10" ht="15" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>

</xml_diff>